<commit_message>
add data 23 Marzo
</commit_message>
<xml_diff>
--- a/datos_brutos.xlsx
+++ b/datos_brutos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="16">
   <si>
     <t>Provincia</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Altas</t>
+  </si>
+  <si>
+    <t>Curados</t>
   </si>
 </sst>
 </file>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +432,7 @@
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -451,8 +454,11 @@
       <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43902</v>
       </c>
@@ -463,7 +469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43902</v>
       </c>
@@ -474,7 +480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43902</v>
       </c>
@@ -485,7 +491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43902</v>
       </c>
@@ -496,7 +502,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43902</v>
       </c>
@@ -507,7 +513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43902</v>
       </c>
@@ -518,7 +524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43902</v>
       </c>
@@ -529,7 +535,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43902</v>
       </c>
@@ -540,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43903</v>
       </c>
@@ -563,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43903</v>
       </c>
@@ -586,7 +592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43903</v>
       </c>
@@ -609,7 +615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43903</v>
       </c>
@@ -632,7 +638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43903</v>
       </c>
@@ -655,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43903</v>
       </c>
@@ -678,7 +684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43903</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43911</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43912</v>
       </c>
@@ -2144,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43912</v>
       </c>
@@ -2164,7 +2170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43912</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43912</v>
       </c>
@@ -2204,7 +2210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43912</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43912</v>
       </c>
@@ -2244,7 +2250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43912</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>43912</v>
       </c>
@@ -2282,6 +2288,214 @@
       </c>
       <c r="F89">
         <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>74</v>
+      </c>
+      <c r="D90">
+        <v>23</v>
+      </c>
+      <c r="E90">
+        <v>49</v>
+      </c>
+      <c r="F90">
+        <v>2</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B91" t="s">
+        <v>2</v>
+      </c>
+      <c r="C91">
+        <v>178</v>
+      </c>
+      <c r="D91">
+        <v>50</v>
+      </c>
+      <c r="E91">
+        <v>125</v>
+      </c>
+      <c r="F91">
+        <v>3</v>
+      </c>
+      <c r="G91">
+        <v>6</v>
+      </c>
+      <c r="H91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92">
+        <v>191</v>
+      </c>
+      <c r="D92">
+        <v>50</v>
+      </c>
+      <c r="E92">
+        <v>137</v>
+      </c>
+      <c r="F92">
+        <v>4</v>
+      </c>
+      <c r="G92">
+        <v>7</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93">
+        <v>374</v>
+      </c>
+      <c r="D93">
+        <v>169</v>
+      </c>
+      <c r="E93">
+        <v>188</v>
+      </c>
+      <c r="F93">
+        <v>17</v>
+      </c>
+      <c r="G93">
+        <v>18</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B94" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <v>58</v>
+      </c>
+      <c r="D94">
+        <v>29</v>
+      </c>
+      <c r="E94">
+        <v>28</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B95" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95">
+        <v>215</v>
+      </c>
+      <c r="D95">
+        <v>79</v>
+      </c>
+      <c r="E95">
+        <v>131</v>
+      </c>
+      <c r="F95">
+        <v>5</v>
+      </c>
+      <c r="G95">
+        <v>12</v>
+      </c>
+      <c r="H95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96">
+        <v>520</v>
+      </c>
+      <c r="D96">
+        <v>192</v>
+      </c>
+      <c r="E96">
+        <v>307</v>
+      </c>
+      <c r="F96">
+        <v>21</v>
+      </c>
+      <c r="G96">
+        <v>44</v>
+      </c>
+      <c r="H96">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97">
+        <v>351</v>
+      </c>
+      <c r="D97">
+        <v>152</v>
+      </c>
+      <c r="E97">
+        <v>194</v>
+      </c>
+      <c r="F97">
+        <v>5</v>
+      </c>
+      <c r="G97">
+        <v>13</v>
+      </c>
+      <c r="H97">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add leaflet map of cases per district
</commit_message>
<xml_diff>
--- a/datos_brutos.xlsx
+++ b/datos_brutos.xlsx
@@ -4,18 +4,38 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="1" r:id="rId1"/>
     <sheet name="test-Andal" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="distritos" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="distri" localSheetId="3">distritos!$A$1:$D$34</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="distri" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr sourceFile="C:\Users\FRS\Dropbox\Rcode\myRcode\researchprojects\COVID19-Andalucia\distri.txt">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="95">
   <si>
     <t>Provincia</t>
   </si>
@@ -87,6 +107,219 @@
   </si>
   <si>
     <t>Curadas.acum</t>
+  </si>
+  <si>
+    <t>Distritos y Área de Gestión Sanitaria</t>
+  </si>
+  <si>
+    <t>Número de casos</t>
+  </si>
+  <si>
+    <t>D. Campo de Cadiz (AGS Campo de Gibraltar)</t>
+  </si>
+  <si>
+    <t>D. Sevilla Este (AGS Osuna)</t>
+  </si>
+  <si>
+    <t>D. Almería Norte (AGS Norte de Almería)</t>
+  </si>
+  <si>
+    <t>D. Córdoba Norte (AGS Norte de Córdoba)</t>
+  </si>
+  <si>
+    <t>D.La Vega (AGS Norte de Málaga)</t>
+  </si>
+  <si>
+    <t>D.Serranía de Málaga (AGS Serranía de Málaga)</t>
+  </si>
+  <si>
+    <t>D.Granada Sur (AGS Sur de Granada)</t>
+  </si>
+  <si>
+    <t>D.Axarquía (AGS Este de Málaga-Axarquía)</t>
+  </si>
+  <si>
+    <t>D.Granada Nordeste (AGS Nordeste de Granada)</t>
+  </si>
+  <si>
+    <t>D.Sierra de Huelva-Andévalo Central (AGS Norte de Huelva)</t>
+  </si>
+  <si>
+    <t>D. Córdoba Sur (AGS Sur de Córdoba)</t>
+  </si>
+  <si>
+    <t>D. Sevilla Sur (AGS Sur de Sevilla)</t>
+  </si>
+  <si>
+    <t>D. Aljarafe</t>
+  </si>
+  <si>
+    <t>D. Almería</t>
+  </si>
+  <si>
+    <t>D. Bahía de Cádiz-La Janda</t>
+  </si>
+  <si>
+    <t>D. Condado-Campiña</t>
+  </si>
+  <si>
+    <t>D. Córdoba</t>
+  </si>
+  <si>
+    <t>D. Costa del Sol</t>
+  </si>
+  <si>
+    <t>D. Granada</t>
+  </si>
+  <si>
+    <t>D.Guadalquivir</t>
+  </si>
+  <si>
+    <t>D.Huelva-Costa</t>
+  </si>
+  <si>
+    <t>D. Jaén</t>
+  </si>
+  <si>
+    <t>D.Jaén Nordeste (AGS Norte de Jaén)</t>
+  </si>
+  <si>
+    <t>D. Jaén Norte (AGS Norte de Jaén)</t>
+  </si>
+  <si>
+    <t>D. Jaén Sur</t>
+  </si>
+  <si>
+    <t>D. Jerez-Costa Noroeste (AGS Norte de Cádiz)</t>
+  </si>
+  <si>
+    <t>D.Málaga</t>
+  </si>
+  <si>
+    <t>D. Metropolitano de Granada</t>
+  </si>
+  <si>
+    <t>D. Poniente de Almería</t>
+  </si>
+  <si>
+    <t>D.Sevilla</t>
+  </si>
+  <si>
+    <t>D. Sevilla Norte</t>
+  </si>
+  <si>
+    <t>D. Sierra de Cádiz (AGS Norte de Cádiz)</t>
+  </si>
+  <si>
+    <t>D.Valle del Guadalhorce</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>CODIST</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>provincia</t>
+  </si>
+  <si>
+    <t>coprov</t>
+  </si>
+  <si>
+    <t>Aljarafe</t>
+  </si>
+  <si>
+    <t>Axarquía</t>
+  </si>
+  <si>
+    <t>Bahía de Cádiz-La Janda</t>
+  </si>
+  <si>
+    <t>Campo de Gibraltar</t>
+  </si>
+  <si>
+    <t>Condado-Campiña</t>
+  </si>
+  <si>
+    <t>Córdoba Norte</t>
+  </si>
+  <si>
+    <t>Córdoba Sur</t>
+  </si>
+  <si>
+    <t>Costa del Sol</t>
+  </si>
+  <si>
+    <t>Granada Nordeste</t>
+  </si>
+  <si>
+    <t>Granada Sur</t>
+  </si>
+  <si>
+    <t>Guadalquivir</t>
+  </si>
+  <si>
+    <t>Huelva-Costa</t>
+  </si>
+  <si>
+    <t>Jaén Nordeste</t>
+  </si>
+  <si>
+    <t>Jaén Norte</t>
+  </si>
+  <si>
+    <t>Jaén Sur</t>
+  </si>
+  <si>
+    <t>Jerez-Costa Noroeste</t>
+  </si>
+  <si>
+    <t>La Vega</t>
+  </si>
+  <si>
+    <t>Levante-Alto Almanzora</t>
+  </si>
+  <si>
+    <t>Metropolitano de Granada</t>
+  </si>
+  <si>
+    <t>Poniente de Almeria</t>
+  </si>
+  <si>
+    <t>Serranía</t>
+  </si>
+  <si>
+    <t>Sevilla Este</t>
+  </si>
+  <si>
+    <t>Sevilla Norte</t>
+  </si>
+  <si>
+    <t>Sevilla Sur</t>
+  </si>
+  <si>
+    <t>Sierra de Cádiz</t>
+  </si>
+  <si>
+    <t>Sierra de Huelva-Andévalo Central</t>
+  </si>
+  <si>
+    <t>Valle del Guadalhorce</t>
+  </si>
+  <si>
+    <t>casos</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>Sumar 112 AN?</t>
+  </si>
+  <si>
+    <t>notas</t>
   </si>
 </sst>
 </file>
@@ -113,12 +346,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -133,12 +372,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,6 +391,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="distri" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A193" activePane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="600" topLeftCell="A190" activePane="bottomLeft"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="D209" sqref="D209"/>
     </sheetView>
@@ -5608,4 +5852,1010 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3004</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3005</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3012</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3013</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F5">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F6">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3022</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3020</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F8">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3049</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F9">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3043</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F10">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3026</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F11">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3046</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F12">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3029</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F13">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3023</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F14">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3048</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3030</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F16">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3031</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>23</v>
+      </c>
+      <c r="E17" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F17">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3045</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F18">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3034</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>23</v>
+      </c>
+      <c r="E19" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F19">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3001</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F20">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3032</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F21">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3011</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>29</v>
+      </c>
+      <c r="E22" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F22">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3033</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F23">
+        <v>67</v>
+      </c>
+      <c r="G23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3028</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>29</v>
+      </c>
+      <c r="E24" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F24">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3056</v>
+      </c>
+      <c r="B25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F25">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3050</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F26">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3052</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>29</v>
+      </c>
+      <c r="E27" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F27">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3057</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>41</v>
+      </c>
+      <c r="E28" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F28">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3047</v>
+      </c>
+      <c r="B29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>41</v>
+      </c>
+      <c r="E29" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F29">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3051</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30">
+        <v>41</v>
+      </c>
+      <c r="E30" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F30">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3002</v>
+      </c>
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31">
+        <v>41</v>
+      </c>
+      <c r="E31" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F31">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3062</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>11</v>
+      </c>
+      <c r="E32" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F32">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3009</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>21</v>
+      </c>
+      <c r="E33" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F33">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3021</v>
+      </c>
+      <c r="B34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>29</v>
+      </c>
+      <c r="E34" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F34">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixing some errors in raw data as provided by Junta de Andalucia
</commit_message>
<xml_diff>
--- a/datos_brutos.xlsx
+++ b/datos_brutos.xlsx
@@ -687,9 +687,9 @@
   <dimension ref="A1:K265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A253" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A220" activePane="bottomLeft"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A266" sqref="A266"/>
+      <selection pane="bottomLeft" activeCell="K232" sqref="K232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4447,7 +4447,7 @@
         <v>89</v>
       </c>
       <c r="I161">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5799,7 +5799,7 @@
         <v>385</v>
       </c>
       <c r="E219">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G219">
         <v>36</v>
@@ -5851,7 +5851,7 @@
         <v>138</v>
       </c>
       <c r="I221">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -6058,7 +6058,7 @@
         <v>21</v>
       </c>
       <c r="I230">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
@@ -6417,7 +6417,7 @@
         <v>318</v>
       </c>
       <c r="D246">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E246">
         <v>27</v>
@@ -6512,10 +6512,10 @@
         <v>176</v>
       </c>
       <c r="E250">
+        <v>34</v>
+      </c>
+      <c r="G250">
         <v>35</v>
-      </c>
-      <c r="G250">
-        <v>36</v>
       </c>
       <c r="I250">
         <v>85</v>
@@ -6879,8 +6879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7631,7 +7631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update 16 Abril. Almeria reduce nº curados en 10 personas!
</commit_message>
<xml_diff>
--- a/datos_brutos.xlsx
+++ b/datos_brutos.xlsx
@@ -4,13 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="datos" sheetId="1" r:id="rId1"/>
     <sheet name="test-Andal" sheetId="2" r:id="rId2"/>
     <sheet name="distritos-raw" sheetId="3" r:id="rId3"/>
     <sheet name="distritos" sheetId="4" r:id="rId4"/>
+    <sheet name="Pred_metadata" sheetId="6" r:id="rId5"/>
+    <sheet name="Pred_And_Confirmados" sheetId="5" r:id="rId6"/>
+    <sheet name="Pred_And_Fallecidos" sheetId="7" r:id="rId7"/>
+    <sheet name="Pred_And_Hospitalizados" sheetId="8" r:id="rId8"/>
+    <sheet name="Pred_And_Nuevos" sheetId="9" r:id="rId9"/>
+    <sheet name="Pred_And_UCI" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="distri" localSheetId="3">distritos!$A$1:$D$34</definedName>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="109">
   <si>
     <t>Provincia</t>
   </si>
@@ -323,6 +329,45 @@
   </si>
   <si>
     <t>Incluye positivos en test rapidos (a diferencia de Ministerio): https://www.juntadeandalucia.es/organismos/saludyfamilias/actualidad/noticias/detalle/234496.html</t>
+  </si>
+  <si>
+    <t>CP01</t>
+  </si>
+  <si>
+    <t>CP02</t>
+  </si>
+  <si>
+    <t>CP03</t>
+  </si>
+  <si>
+    <t>CP04</t>
+  </si>
+  <si>
+    <t>CP05</t>
+  </si>
+  <si>
+    <t>CP06</t>
+  </si>
+  <si>
+    <t>CP07</t>
+  </si>
+  <si>
+    <t>npre</t>
+  </si>
+  <si>
+    <t>nphis</t>
+  </si>
+  <si>
+    <t>ndhis</t>
+  </si>
+  <si>
+    <t>CP01 :Simple Average, CP02: Median, CP03: Trimmed Mean, CP04: Winsored Mean, CP05: Bates/Granger(mod), CP06: Lowess, CP07: Loess+Bates/Granger(mod), npre: Número de predictores individuales, nphis: Número de predictores individuales en el histórico para el entrenamiento de CP06 y CP08, ndhis: Número (máximo) de observaciones en el histórico</t>
+  </si>
+  <si>
+    <t>fecha-captura</t>
+  </si>
+  <si>
+    <t>row</t>
   </si>
 </sst>
 </file>
@@ -687,12 +732,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K281"/>
+  <dimension ref="A1:K289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A262" activePane="bottomLeft"/>
+      <pane ySplit="600" topLeftCell="A274" activePane="bottomLeft"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="B280" sqref="B280"/>
+      <selection pane="bottomLeft" activeCell="B289" sqref="B282:B289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7240,6 +7285,190 @@
         <v>327</v>
       </c>
     </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1</v>
+      </c>
+      <c r="C282">
+        <v>428</v>
+      </c>
+      <c r="D282">
+        <v>181</v>
+      </c>
+      <c r="E282">
+        <v>35</v>
+      </c>
+      <c r="G282">
+        <v>38</v>
+      </c>
+      <c r="I282">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B283" t="s">
+        <v>2</v>
+      </c>
+      <c r="C283">
+        <v>1072</v>
+      </c>
+      <c r="D283">
+        <v>460</v>
+      </c>
+      <c r="E283">
+        <v>71</v>
+      </c>
+      <c r="G283">
+        <v>68</v>
+      </c>
+      <c r="I283">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B284" t="s">
+        <v>3</v>
+      </c>
+      <c r="C284">
+        <v>1247</v>
+      </c>
+      <c r="D284">
+        <v>479</v>
+      </c>
+      <c r="E284">
+        <v>62</v>
+      </c>
+      <c r="G284">
+        <v>63</v>
+      </c>
+      <c r="I284">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B285" t="s">
+        <v>4</v>
+      </c>
+      <c r="C285">
+        <v>1926</v>
+      </c>
+      <c r="D285">
+        <v>1004</v>
+      </c>
+      <c r="E285">
+        <v>117</v>
+      </c>
+      <c r="G285">
+        <v>187</v>
+      </c>
+      <c r="I285">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B286" t="s">
+        <v>11</v>
+      </c>
+      <c r="C286">
+        <v>347</v>
+      </c>
+      <c r="D286">
+        <v>200</v>
+      </c>
+      <c r="E286">
+        <v>30</v>
+      </c>
+      <c r="G286">
+        <v>28</v>
+      </c>
+      <c r="I286">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B287" t="s">
+        <v>5</v>
+      </c>
+      <c r="C287">
+        <v>1201</v>
+      </c>
+      <c r="D287">
+        <v>608</v>
+      </c>
+      <c r="E287">
+        <v>62</v>
+      </c>
+      <c r="G287">
+        <v>128</v>
+      </c>
+      <c r="I287">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B288" t="s">
+        <v>6</v>
+      </c>
+      <c r="C288">
+        <v>2363</v>
+      </c>
+      <c r="D288">
+        <v>1302</v>
+      </c>
+      <c r="E288">
+        <v>156</v>
+      </c>
+      <c r="G288">
+        <v>211</v>
+      </c>
+      <c r="I288">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B289" t="s">
+        <v>7</v>
+      </c>
+      <c r="C289">
+        <v>2223</v>
+      </c>
+      <c r="D289">
+        <v>992</v>
+      </c>
+      <c r="E289">
+        <v>138</v>
+      </c>
+      <c r="G289">
+        <v>189</v>
+      </c>
+      <c r="I289">
+        <v>402</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:G57">
     <sortCondition ref="A1"/>
@@ -7249,12 +7478,361 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C2">
+        <v>650</v>
+      </c>
+      <c r="D2">
+        <v>646</v>
+      </c>
+      <c r="E2">
+        <v>649</v>
+      </c>
+      <c r="F2">
+        <v>653</v>
+      </c>
+      <c r="G2">
+        <v>648</v>
+      </c>
+      <c r="H2">
+        <v>651</v>
+      </c>
+      <c r="I2">
+        <v>649</v>
+      </c>
+      <c r="J2">
+        <v>11</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C3">
+        <v>661</v>
+      </c>
+      <c r="D3">
+        <v>660</v>
+      </c>
+      <c r="E3">
+        <v>659</v>
+      </c>
+      <c r="F3">
+        <v>662</v>
+      </c>
+      <c r="G3">
+        <v>660</v>
+      </c>
+      <c r="H3">
+        <v>658</v>
+      </c>
+      <c r="I3">
+        <v>659</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43937</v>
+      </c>
+      <c r="C4">
+        <v>671</v>
+      </c>
+      <c r="D4">
+        <v>668</v>
+      </c>
+      <c r="E4">
+        <v>666</v>
+      </c>
+      <c r="F4">
+        <v>668</v>
+      </c>
+      <c r="G4">
+        <v>669</v>
+      </c>
+      <c r="H4">
+        <v>664</v>
+      </c>
+      <c r="I4">
+        <v>669</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C5">
+        <v>681</v>
+      </c>
+      <c r="D5">
+        <v>677</v>
+      </c>
+      <c r="E5">
+        <v>672</v>
+      </c>
+      <c r="F5">
+        <v>673</v>
+      </c>
+      <c r="G5">
+        <v>678</v>
+      </c>
+      <c r="H5">
+        <v>666</v>
+      </c>
+      <c r="I5">
+        <v>677</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C6">
+        <v>691</v>
+      </c>
+      <c r="D6">
+        <v>685</v>
+      </c>
+      <c r="E6">
+        <v>678</v>
+      </c>
+      <c r="F6">
+        <v>677</v>
+      </c>
+      <c r="G6">
+        <v>688</v>
+      </c>
+      <c r="H6">
+        <v>672</v>
+      </c>
+      <c r="I6">
+        <v>691</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43940</v>
+      </c>
+      <c r="C7">
+        <v>716</v>
+      </c>
+      <c r="D7">
+        <v>702</v>
+      </c>
+      <c r="E7">
+        <v>697</v>
+      </c>
+      <c r="F7">
+        <v>695</v>
+      </c>
+      <c r="G7">
+        <v>710</v>
+      </c>
+      <c r="H7">
+        <v>681</v>
+      </c>
+      <c r="I7">
+        <v>706</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C8">
+        <v>730</v>
+      </c>
+      <c r="D8">
+        <v>711</v>
+      </c>
+      <c r="E8">
+        <v>702</v>
+      </c>
+      <c r="F8">
+        <v>699</v>
+      </c>
+      <c r="G8">
+        <v>721</v>
+      </c>
+      <c r="H8">
+        <v>690</v>
+      </c>
+      <c r="I8">
+        <v>722</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D20" sqref="D20:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7718,6 +8296,29 @@
       <c r="F20">
         <f t="shared" ref="F20" si="41">E20/D20</f>
         <v>0.22900158478605387</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B21">
+        <v>44598</v>
+      </c>
+      <c r="C21">
+        <v>10807</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21" si="42">B21-B20</f>
+        <v>973</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" si="43">C21-C20</f>
+        <v>212</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21" si="44">E21/D21</f>
+        <v>0.21788283658787255</v>
       </c>
     </row>
   </sheetData>
@@ -8730,4 +9331,1420 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C2">
+        <v>10334</v>
+      </c>
+      <c r="D2">
+        <v>10282</v>
+      </c>
+      <c r="E2">
+        <v>10316</v>
+      </c>
+      <c r="F2">
+        <v>10322</v>
+      </c>
+      <c r="G2">
+        <v>10331</v>
+      </c>
+      <c r="H2">
+        <v>10343</v>
+      </c>
+      <c r="I2">
+        <v>10334</v>
+      </c>
+      <c r="J2">
+        <v>13</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C3">
+        <v>10450</v>
+      </c>
+      <c r="D3">
+        <v>10375</v>
+      </c>
+      <c r="E3">
+        <v>10436</v>
+      </c>
+      <c r="F3">
+        <v>10442</v>
+      </c>
+      <c r="G3">
+        <v>10445</v>
+      </c>
+      <c r="H3">
+        <v>10426</v>
+      </c>
+      <c r="I3">
+        <v>10438</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43937</v>
+      </c>
+      <c r="C4">
+        <v>10525</v>
+      </c>
+      <c r="D4">
+        <v>10426</v>
+      </c>
+      <c r="E4">
+        <v>10493</v>
+      </c>
+      <c r="F4">
+        <v>10497</v>
+      </c>
+      <c r="G4">
+        <v>10523</v>
+      </c>
+      <c r="H4">
+        <v>10505</v>
+      </c>
+      <c r="I4">
+        <v>10525</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C5">
+        <v>10600</v>
+      </c>
+      <c r="D5">
+        <v>10480</v>
+      </c>
+      <c r="E5">
+        <v>10568</v>
+      </c>
+      <c r="F5">
+        <v>10572</v>
+      </c>
+      <c r="G5">
+        <v>10594</v>
+      </c>
+      <c r="H5">
+        <v>10554</v>
+      </c>
+      <c r="I5">
+        <v>10597</v>
+      </c>
+      <c r="J5">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C6">
+        <v>10670</v>
+      </c>
+      <c r="D6">
+        <v>10533</v>
+      </c>
+      <c r="E6">
+        <v>10636</v>
+      </c>
+      <c r="F6">
+        <v>10648</v>
+      </c>
+      <c r="G6">
+        <v>10663</v>
+      </c>
+      <c r="H6">
+        <v>10571</v>
+      </c>
+      <c r="I6">
+        <v>10658</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43940</v>
+      </c>
+      <c r="C7">
+        <v>10704</v>
+      </c>
+      <c r="D7">
+        <v>10566</v>
+      </c>
+      <c r="E7">
+        <v>10630</v>
+      </c>
+      <c r="F7">
+        <v>10652</v>
+      </c>
+      <c r="G7">
+        <v>10701</v>
+      </c>
+      <c r="H7">
+        <v>10563</v>
+      </c>
+      <c r="I7">
+        <v>10705</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C8">
+        <v>10759</v>
+      </c>
+      <c r="D8">
+        <v>10594</v>
+      </c>
+      <c r="E8">
+        <v>10666</v>
+      </c>
+      <c r="F8">
+        <v>10694</v>
+      </c>
+      <c r="G8">
+        <v>10737</v>
+      </c>
+      <c r="H8">
+        <v>10554</v>
+      </c>
+      <c r="I8">
+        <v>10736</v>
+      </c>
+      <c r="J8">
+        <v>11</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C2">
+        <v>870</v>
+      </c>
+      <c r="D2">
+        <v>870</v>
+      </c>
+      <c r="E2">
+        <v>870</v>
+      </c>
+      <c r="F2">
+        <v>870</v>
+      </c>
+      <c r="G2">
+        <v>870</v>
+      </c>
+      <c r="H2">
+        <v>871</v>
+      </c>
+      <c r="I2">
+        <v>870</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C3">
+        <v>900</v>
+      </c>
+      <c r="D3">
+        <v>899</v>
+      </c>
+      <c r="E3">
+        <v>900</v>
+      </c>
+      <c r="F3">
+        <v>901</v>
+      </c>
+      <c r="G3">
+        <v>900</v>
+      </c>
+      <c r="H3">
+        <v>899</v>
+      </c>
+      <c r="I3">
+        <v>899</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43937</v>
+      </c>
+      <c r="C4">
+        <v>925</v>
+      </c>
+      <c r="D4">
+        <v>926</v>
+      </c>
+      <c r="E4">
+        <v>925</v>
+      </c>
+      <c r="F4">
+        <v>926</v>
+      </c>
+      <c r="G4">
+        <v>923</v>
+      </c>
+      <c r="H4">
+        <v>926</v>
+      </c>
+      <c r="I4">
+        <v>923</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C5">
+        <v>951</v>
+      </c>
+      <c r="D5">
+        <v>954</v>
+      </c>
+      <c r="E5">
+        <v>952</v>
+      </c>
+      <c r="F5">
+        <v>952</v>
+      </c>
+      <c r="G5">
+        <v>949</v>
+      </c>
+      <c r="H5">
+        <v>951</v>
+      </c>
+      <c r="I5">
+        <v>949</v>
+      </c>
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C6">
+        <v>977</v>
+      </c>
+      <c r="D6">
+        <v>979</v>
+      </c>
+      <c r="E6">
+        <v>977</v>
+      </c>
+      <c r="F6">
+        <v>978</v>
+      </c>
+      <c r="G6">
+        <v>975</v>
+      </c>
+      <c r="H6">
+        <v>975</v>
+      </c>
+      <c r="I6">
+        <v>975</v>
+      </c>
+      <c r="J6">
+        <v>11</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43940</v>
+      </c>
+      <c r="C7">
+        <v>1001</v>
+      </c>
+      <c r="D7">
+        <v>996</v>
+      </c>
+      <c r="E7">
+        <v>998</v>
+      </c>
+      <c r="F7">
+        <v>999</v>
+      </c>
+      <c r="G7">
+        <v>997</v>
+      </c>
+      <c r="H7">
+        <v>997</v>
+      </c>
+      <c r="I7">
+        <v>998</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C8">
+        <v>1025</v>
+      </c>
+      <c r="D8">
+        <v>1015</v>
+      </c>
+      <c r="E8">
+        <v>1019</v>
+      </c>
+      <c r="F8">
+        <v>1020</v>
+      </c>
+      <c r="G8">
+        <v>1020</v>
+      </c>
+      <c r="H8">
+        <v>1019</v>
+      </c>
+      <c r="I8">
+        <v>1019</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C2">
+        <v>5123</v>
+      </c>
+      <c r="D2">
+        <v>5092</v>
+      </c>
+      <c r="E2">
+        <v>5088</v>
+      </c>
+      <c r="F2">
+        <v>5086</v>
+      </c>
+      <c r="G2">
+        <v>5082</v>
+      </c>
+      <c r="H2">
+        <v>5090</v>
+      </c>
+      <c r="I2">
+        <v>5082</v>
+      </c>
+      <c r="J2">
+        <v>11</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C3">
+        <v>5184</v>
+      </c>
+      <c r="D3">
+        <v>5133</v>
+      </c>
+      <c r="E3">
+        <v>5122</v>
+      </c>
+      <c r="F3">
+        <v>5120</v>
+      </c>
+      <c r="G3">
+        <v>5112</v>
+      </c>
+      <c r="H3">
+        <v>5112</v>
+      </c>
+      <c r="I3">
+        <v>5110</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43937</v>
+      </c>
+      <c r="C4">
+        <v>5242</v>
+      </c>
+      <c r="D4">
+        <v>5137</v>
+      </c>
+      <c r="E4">
+        <v>5137</v>
+      </c>
+      <c r="F4">
+        <v>5135</v>
+      </c>
+      <c r="G4">
+        <v>5121</v>
+      </c>
+      <c r="H4">
+        <v>5133</v>
+      </c>
+      <c r="I4">
+        <v>5121</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C5">
+        <v>5304</v>
+      </c>
+      <c r="D5">
+        <v>5154</v>
+      </c>
+      <c r="E5">
+        <v>5146</v>
+      </c>
+      <c r="F5">
+        <v>5140</v>
+      </c>
+      <c r="G5">
+        <v>5124</v>
+      </c>
+      <c r="H5">
+        <v>5142</v>
+      </c>
+      <c r="I5">
+        <v>5123</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C6">
+        <v>5384</v>
+      </c>
+      <c r="D6">
+        <v>5167</v>
+      </c>
+      <c r="E6">
+        <v>5155</v>
+      </c>
+      <c r="F6">
+        <v>5151</v>
+      </c>
+      <c r="G6">
+        <v>5130</v>
+      </c>
+      <c r="H6">
+        <v>5157</v>
+      </c>
+      <c r="I6">
+        <v>5137</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43940</v>
+      </c>
+      <c r="C7">
+        <v>5541</v>
+      </c>
+      <c r="D7">
+        <v>5221</v>
+      </c>
+      <c r="E7">
+        <v>5177</v>
+      </c>
+      <c r="F7">
+        <v>5173</v>
+      </c>
+      <c r="G7">
+        <v>5164</v>
+      </c>
+      <c r="H7">
+        <v>5176</v>
+      </c>
+      <c r="I7">
+        <v>5153</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C8">
+        <v>5686</v>
+      </c>
+      <c r="D8">
+        <v>5218</v>
+      </c>
+      <c r="E8">
+        <v>5181</v>
+      </c>
+      <c r="F8">
+        <v>5179</v>
+      </c>
+      <c r="G8">
+        <v>5163</v>
+      </c>
+      <c r="H8">
+        <v>5195</v>
+      </c>
+      <c r="I8">
+        <v>5167</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43935</v>
+      </c>
+      <c r="C2">
+        <v>122</v>
+      </c>
+      <c r="D2">
+        <v>96</v>
+      </c>
+      <c r="E2">
+        <v>108</v>
+      </c>
+      <c r="F2">
+        <v>117</v>
+      </c>
+      <c r="G2">
+        <v>116</v>
+      </c>
+      <c r="H2">
+        <v>102</v>
+      </c>
+      <c r="I2">
+        <v>119</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43936</v>
+      </c>
+      <c r="C3">
+        <v>120</v>
+      </c>
+      <c r="D3">
+        <v>87</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>106</v>
+      </c>
+      <c r="G3">
+        <v>116</v>
+      </c>
+      <c r="H3">
+        <v>91</v>
+      </c>
+      <c r="I3">
+        <v>108</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43937</v>
+      </c>
+      <c r="C4">
+        <v>95</v>
+      </c>
+      <c r="D4">
+        <v>74</v>
+      </c>
+      <c r="E4">
+        <v>84</v>
+      </c>
+      <c r="F4">
+        <v>88</v>
+      </c>
+      <c r="G4">
+        <v>88</v>
+      </c>
+      <c r="H4">
+        <v>81</v>
+      </c>
+      <c r="I4">
+        <v>90</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43938</v>
+      </c>
+      <c r="C5">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>64</v>
+      </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>70</v>
+      </c>
+      <c r="G5">
+        <v>66</v>
+      </c>
+      <c r="H5">
+        <v>70</v>
+      </c>
+      <c r="I5">
+        <v>66</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43939</v>
+      </c>
+      <c r="C6">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>55</v>
+      </c>
+      <c r="E6">
+        <v>57</v>
+      </c>
+      <c r="F6">
+        <v>58</v>
+      </c>
+      <c r="G6">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>58</v>
+      </c>
+      <c r="I6">
+        <v>56</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>43940</v>
+      </c>
+      <c r="C7">
+        <v>61</v>
+      </c>
+      <c r="D7">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <v>47</v>
+      </c>
+      <c r="G7">
+        <v>52</v>
+      </c>
+      <c r="H7">
+        <v>45</v>
+      </c>
+      <c r="I7">
+        <v>49</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43941</v>
+      </c>
+      <c r="C8">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>38</v>
+      </c>
+      <c r="G8">
+        <v>43</v>
+      </c>
+      <c r="H8">
+        <v>32</v>
+      </c>
+      <c r="I8">
+        <v>44</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1">
+        <v>43936</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cambio fechas un dia menos (dia de los datos, no del informe). Cambio Curadas Almeria para que no haya descenso
</commit_message>
<xml_diff>
--- a/datos_brutos.xlsx
+++ b/datos_brutos.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="109">
   <si>
     <t>Provincia</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>Notas</t>
-  </si>
-  <si>
-    <t>Fuente: https://twitter.com/JuanMa_Moreno</t>
   </si>
   <si>
     <t>Ntest.acum</t>
@@ -325,9 +322,6 @@
     <t>notas</t>
   </si>
   <si>
-    <t>https://twitter.com/AndaluciaJunta/status/1247466253683482624?s=20</t>
-  </si>
-  <si>
     <t>Incluye positivos en test rapidos (a diferencia de Ministerio): https://www.juntadeandalucia.es/organismos/saludyfamilias/actualidad/noticias/detalle/234496.html</t>
   </si>
   <si>
@@ -368,6 +362,12 @@
   </si>
   <si>
     <t>row</t>
+  </si>
+  <si>
+    <t>Fuente: https://twitter.com/AndaluciaJunta</t>
+  </si>
+  <si>
+    <t>Vease tambien  https://docs.google.com/spreadsheets/d/1U-PFh3VmXAs1rgGxTNHkFtlPoM-ZyEGG_chtYdlLoyI/edit#gid=0</t>
   </si>
 </sst>
 </file>
@@ -732,12 +732,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K289"/>
+  <dimension ref="A1:K297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="600" topLeftCell="A274" activePane="bottomLeft"/>
-      <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="B289" sqref="B282:B289"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="I283" sqref="I283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,10 +762,10 @@
         <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>12</v>
@@ -774,13 +774,13 @@
         <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>13</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="3" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="4" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
@@ -865,7 +865,7 @@
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43902</v>
+        <v>43901</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>1</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="11" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>2</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="12" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>4</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>11</v>
@@ -996,7 +996,7 @@
     </row>
     <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>5</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>6</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43903</v>
+        <v>43902</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
@@ -1114,7 +1114,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B21" t="s">
         <v>4</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>43904</v>
+        <v>43903</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B28" t="s">
         <v>3</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -1390,7 +1390,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43905</v>
+        <v>43904</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>43906</v>
+        <v>43905</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B42" t="s">
         <v>1</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B43" t="s">
         <v>2</v>
@@ -1666,7 +1666,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B44" t="s">
         <v>3</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B45" t="s">
         <v>4</v>
@@ -1712,7 +1712,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B46" t="s">
         <v>11</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B48" t="s">
         <v>6</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>43907</v>
+        <v>43906</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B50" t="s">
         <v>1</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
@@ -1850,7 +1850,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B52" t="s">
         <v>3</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B53" t="s">
         <v>4</v>
@@ -1896,7 +1896,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B54" t="s">
         <v>11</v>
@@ -1919,7 +1919,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>43908</v>
+        <v>43907</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B58" t="s">
         <v>1</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B59" t="s">
         <v>2</v>
@@ -2028,7 +2028,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B61" t="s">
         <v>4</v>
@@ -2068,7 +2068,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
@@ -2088,7 +2088,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B63" t="s">
         <v>5</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -2128,7 +2128,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>43909</v>
+        <v>43908</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B67" t="s">
         <v>2</v>
@@ -2188,7 +2188,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B68" t="s">
         <v>3</v>
@@ -2208,7 +2208,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B69" t="s">
         <v>4</v>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -2288,7 +2288,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>43910</v>
+        <v>43909</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -2308,7 +2308,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B75" t="s">
         <v>2</v>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B76" t="s">
         <v>3</v>
@@ -2368,7 +2368,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B77" t="s">
         <v>4</v>
@@ -2388,7 +2388,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
@@ -2408,7 +2408,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B80" t="s">
         <v>6</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>43911</v>
+        <v>43910</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B84" t="s">
         <v>3</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B85" t="s">
         <v>4</v>
@@ -2548,7 +2548,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B86" t="s">
         <v>11</v>
@@ -2568,7 +2568,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>43912</v>
+        <v>43911</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
@@ -2628,7 +2628,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
@@ -2654,7 +2654,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B91" t="s">
         <v>2</v>
@@ -2680,7 +2680,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B92" t="s">
         <v>3</v>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B93" t="s">
         <v>4</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B94" t="s">
         <v>11</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
@@ -2784,7 +2784,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>43913</v>
+        <v>43912</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
@@ -2836,7 +2836,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B99" t="s">
         <v>2</v>
@@ -2888,7 +2888,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B100" t="s">
         <v>3</v>
@@ -2914,7 +2914,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B101" t="s">
         <v>4</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B102" t="s">
         <v>11</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B103" t="s">
         <v>5</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
@@ -3018,7 +3018,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>43914</v>
+        <v>43913</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
@@ -3044,7 +3044,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B106" t="s">
         <v>1</v>
@@ -3070,7 +3070,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B107" t="s">
         <v>2</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B108" t="s">
         <v>3</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B109" t="s">
         <v>4</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B110" t="s">
         <v>11</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B111" t="s">
         <v>5</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
@@ -3226,7 +3226,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>43915</v>
+        <v>43914</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B114" t="s">
         <v>1</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B115" t="s">
         <v>2</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B116" t="s">
         <v>3</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B117" t="s">
         <v>4</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B118" t="s">
         <v>11</v>
@@ -3382,7 +3382,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
@@ -3408,7 +3408,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B121" t="s">
         <v>7</v>
@@ -3460,7 +3460,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B122" t="s">
         <v>1</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B123" t="s">
         <v>2</v>
@@ -3512,7 +3512,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B124" t="s">
         <v>3</v>
@@ -3538,7 +3538,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B125" t="s">
         <v>4</v>
@@ -3564,7 +3564,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B126" t="s">
         <v>11</v>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B127" t="s">
         <v>5</v>
@@ -3616,7 +3616,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B129" t="s">
         <v>7</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B130" t="s">
         <v>1</v>
@@ -3694,7 +3694,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B131" t="s">
         <v>2</v>
@@ -3720,7 +3720,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B132" t="s">
         <v>3</v>
@@ -3746,7 +3746,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B133" t="s">
         <v>4</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B134" t="s">
         <v>11</v>
@@ -3798,7 +3798,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B135" t="s">
         <v>5</v>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B136" t="s">
         <v>6</v>
@@ -3850,7 +3850,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B137" t="s">
         <v>7</v>
@@ -3876,7 +3876,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B138" t="s">
         <v>1</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B139" t="s">
         <v>2</v>
@@ -3928,7 +3928,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B140" t="s">
         <v>3</v>
@@ -3954,7 +3954,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B141" t="s">
         <v>4</v>
@@ -3980,7 +3980,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B142" t="s">
         <v>11</v>
@@ -4006,7 +4006,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B143" t="s">
         <v>5</v>
@@ -4032,7 +4032,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B144" t="s">
         <v>6</v>
@@ -4058,7 +4058,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B145" t="s">
         <v>7</v>
@@ -4084,7 +4084,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B146" t="s">
         <v>1</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B147" t="s">
         <v>2</v>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B148" t="s">
         <v>3</v>
@@ -4162,7 +4162,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B149" t="s">
         <v>4</v>
@@ -4188,7 +4188,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B150" t="s">
         <v>11</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B151" t="s">
         <v>5</v>
@@ -4240,7 +4240,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B152" t="s">
         <v>6</v>
@@ -4266,7 +4266,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B153" t="s">
         <v>7</v>
@@ -4292,7 +4292,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B154" t="s">
         <v>1</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B155" t="s">
         <v>2</v>
@@ -4344,7 +4344,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B156" t="s">
         <v>3</v>
@@ -4370,7 +4370,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B157" t="s">
         <v>4</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B158" t="s">
         <v>11</v>
@@ -4422,7 +4422,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B159" t="s">
         <v>5</v>
@@ -4448,7 +4448,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B160" t="s">
         <v>6</v>
@@ -4474,7 +4474,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B161" t="s">
         <v>7</v>
@@ -4500,7 +4500,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B162" t="s">
         <v>1</v>
@@ -4523,7 +4523,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B163" t="s">
         <v>2</v>
@@ -4546,7 +4546,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B164" t="s">
         <v>3</v>
@@ -4569,7 +4569,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B165" t="s">
         <v>4</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B166" t="s">
         <v>11</v>
@@ -4615,7 +4615,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B167" t="s">
         <v>5</v>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B168" t="s">
         <v>6</v>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B169" t="s">
         <v>7</v>
@@ -4684,7 +4684,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B170" t="s">
         <v>1</v>
@@ -4707,7 +4707,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B171" t="s">
         <v>2</v>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B172" t="s">
         <v>3</v>
@@ -4753,7 +4753,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B173" t="s">
         <v>4</v>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B174" t="s">
         <v>11</v>
@@ -4799,7 +4799,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B175" t="s">
         <v>5</v>
@@ -4822,7 +4822,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B176" t="s">
         <v>6</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B177" t="s">
         <v>7</v>
@@ -4868,7 +4868,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B179" t="s">
         <v>2</v>
@@ -4914,7 +4914,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B180" t="s">
         <v>3</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B181" t="s">
         <v>4</v>
@@ -4960,7 +4960,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B182" t="s">
         <v>11</v>
@@ -4983,7 +4983,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B183" t="s">
         <v>5</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B184" t="s">
         <v>6</v>
@@ -5029,7 +5029,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B185" t="s">
         <v>7</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B186" t="s">
         <v>1</v>
@@ -5078,7 +5078,7 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B187" t="s">
         <v>2</v>
@@ -5104,7 +5104,7 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B188" t="s">
         <v>3</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B189" t="s">
         <v>4</v>
@@ -5156,7 +5156,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B190" t="s">
         <v>11</v>
@@ -5182,7 +5182,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B191" t="s">
         <v>5</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B192" t="s">
         <v>6</v>
@@ -5234,7 +5234,7 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -5260,7 +5260,7 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B194" t="s">
         <v>1</v>
@@ -5283,7 +5283,7 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B195" t="s">
         <v>2</v>
@@ -5306,7 +5306,7 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B196" t="s">
         <v>3</v>
@@ -5329,7 +5329,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B197" t="s">
         <v>4</v>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B198" t="s">
         <v>11</v>
@@ -5375,7 +5375,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B199" t="s">
         <v>5</v>
@@ -5398,7 +5398,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B200" t="s">
         <v>6</v>
@@ -5421,7 +5421,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B201" t="s">
         <v>7</v>
@@ -5444,7 +5444,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B202" t="s">
         <v>1</v>
@@ -5467,7 +5467,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B203" t="s">
         <v>2</v>
@@ -5490,7 +5490,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B204" t="s">
         <v>3</v>
@@ -5513,7 +5513,7 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B205" t="s">
         <v>4</v>
@@ -5536,7 +5536,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B206" t="s">
         <v>11</v>
@@ -5559,7 +5559,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B207" t="s">
         <v>5</v>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B208" t="s">
         <v>6</v>
@@ -5605,7 +5605,7 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B209" t="s">
         <v>7</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B210" t="s">
         <v>1</v>
@@ -5651,7 +5651,7 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B211" t="s">
         <v>2</v>
@@ -5674,7 +5674,7 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B212" t="s">
         <v>3</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B213" t="s">
         <v>4</v>
@@ -5720,7 +5720,7 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B214" t="s">
         <v>11</v>
@@ -5743,7 +5743,7 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B215" t="s">
         <v>5</v>
@@ -5766,7 +5766,7 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B216" t="s">
         <v>6</v>
@@ -5789,7 +5789,7 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>43928</v>
+        <v>43927</v>
       </c>
       <c r="B217" t="s">
         <v>7</v>
@@ -5812,7 +5812,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B218" t="s">
         <v>1</v>
@@ -5835,7 +5835,7 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B219" t="s">
         <v>2</v>
@@ -5858,7 +5858,7 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B220" t="s">
         <v>3</v>
@@ -5881,7 +5881,7 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B221" t="s">
         <v>4</v>
@@ -5904,7 +5904,7 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B222" t="s">
         <v>11</v>
@@ -5927,7 +5927,7 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B223" t="s">
         <v>5</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B224" t="s">
         <v>6</v>
@@ -5973,7 +5973,7 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>43929</v>
+        <v>43928</v>
       </c>
       <c r="B225" t="s">
         <v>7</v>
@@ -5996,7 +5996,7 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B226" t="s">
         <v>1</v>
@@ -6019,7 +6019,7 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B227" t="s">
         <v>2</v>
@@ -6042,7 +6042,7 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B228" t="s">
         <v>3</v>
@@ -6065,7 +6065,7 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B229" t="s">
         <v>4</v>
@@ -6088,7 +6088,7 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B230" t="s">
         <v>11</v>
@@ -6111,7 +6111,7 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B231" t="s">
         <v>5</v>
@@ -6134,7 +6134,7 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B232" t="s">
         <v>6</v>
@@ -6157,7 +6157,7 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>43930</v>
+        <v>43929</v>
       </c>
       <c r="B233" t="s">
         <v>7</v>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B234" t="s">
         <v>1</v>
@@ -6203,7 +6203,7 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B235" t="s">
         <v>2</v>
@@ -6226,7 +6226,7 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B236" t="s">
         <v>3</v>
@@ -6249,7 +6249,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B237" t="s">
         <v>4</v>
@@ -6272,7 +6272,7 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B238" t="s">
         <v>11</v>
@@ -6295,7 +6295,7 @@
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B239" t="s">
         <v>5</v>
@@ -6318,7 +6318,7 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B240" t="s">
         <v>6</v>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>43931</v>
+        <v>43930</v>
       </c>
       <c r="B241" t="s">
         <v>7</v>
@@ -6364,7 +6364,7 @@
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B242" t="s">
         <v>1</v>
@@ -6387,7 +6387,7 @@
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B243" t="s">
         <v>2</v>
@@ -6410,7 +6410,7 @@
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B244" t="s">
         <v>3</v>
@@ -6433,7 +6433,7 @@
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B245" t="s">
         <v>4</v>
@@ -6456,7 +6456,7 @@
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B246" t="s">
         <v>11</v>
@@ -6479,7 +6479,7 @@
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B247" t="s">
         <v>5</v>
@@ -6502,7 +6502,7 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B248" t="s">
         <v>6</v>
@@ -6525,7 +6525,7 @@
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>43932</v>
+        <v>43931</v>
       </c>
       <c r="B249" t="s">
         <v>7</v>
@@ -6548,7 +6548,7 @@
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B250" t="s">
         <v>1</v>
@@ -6571,7 +6571,7 @@
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B251" t="s">
         <v>2</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B252" t="s">
         <v>3</v>
@@ -6617,7 +6617,7 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B253" t="s">
         <v>4</v>
@@ -6640,7 +6640,7 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B254" t="s">
         <v>11</v>
@@ -6663,7 +6663,7 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B255" t="s">
         <v>5</v>
@@ -6686,7 +6686,7 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B256" t="s">
         <v>6</v>
@@ -6709,7 +6709,7 @@
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>43933</v>
+        <v>43932</v>
       </c>
       <c r="B257" t="s">
         <v>7</v>
@@ -6732,7 +6732,7 @@
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B258" t="s">
         <v>1</v>
@@ -6755,7 +6755,7 @@
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B259" t="s">
         <v>2</v>
@@ -6778,7 +6778,7 @@
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B260" t="s">
         <v>3</v>
@@ -6801,7 +6801,7 @@
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B261" t="s">
         <v>4</v>
@@ -6824,7 +6824,7 @@
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B262" t="s">
         <v>11</v>
@@ -6847,7 +6847,7 @@
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B263" t="s">
         <v>5</v>
@@ -6870,7 +6870,7 @@
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B264" t="s">
         <v>6</v>
@@ -6893,7 +6893,7 @@
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>43934</v>
+        <v>43933</v>
       </c>
       <c r="B265" t="s">
         <v>7</v>
@@ -6916,7 +6916,7 @@
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B266" t="s">
         <v>1</v>
@@ -6937,12 +6937,12 @@
         <v>96</v>
       </c>
       <c r="K266" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B267" t="s">
         <v>2</v>
@@ -6965,7 +6965,7 @@
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B268" t="s">
         <v>3</v>
@@ -6988,7 +6988,7 @@
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B269" t="s">
         <v>4</v>
@@ -7011,7 +7011,7 @@
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B270" t="s">
         <v>11</v>
@@ -7034,7 +7034,7 @@
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B271" t="s">
         <v>5</v>
@@ -7057,7 +7057,7 @@
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B272" t="s">
         <v>6</v>
@@ -7080,7 +7080,7 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>43935</v>
+        <v>43934</v>
       </c>
       <c r="B273" t="s">
         <v>7</v>
@@ -7103,7 +7103,7 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B274" t="s">
         <v>1</v>
@@ -7126,7 +7126,7 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B275" t="s">
         <v>2</v>
@@ -7149,7 +7149,7 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B276" t="s">
         <v>3</v>
@@ -7172,7 +7172,7 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B277" t="s">
         <v>4</v>
@@ -7195,7 +7195,7 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B278" t="s">
         <v>11</v>
@@ -7218,7 +7218,7 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B279" t="s">
         <v>5</v>
@@ -7241,7 +7241,7 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B280" t="s">
         <v>6</v>
@@ -7264,7 +7264,7 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
-        <v>43936</v>
+        <v>43935</v>
       </c>
       <c r="B281" t="s">
         <v>7</v>
@@ -7287,7 +7287,7 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B282" t="s">
         <v>1</v>
@@ -7305,12 +7305,12 @@
         <v>38</v>
       </c>
       <c r="I282">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B283" t="s">
         <v>2</v>
@@ -7333,7 +7333,7 @@
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B284" t="s">
         <v>3</v>
@@ -7356,7 +7356,7 @@
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B285" t="s">
         <v>4</v>
@@ -7379,7 +7379,7 @@
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B286" t="s">
         <v>11</v>
@@ -7402,7 +7402,7 @@
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B287" t="s">
         <v>5</v>
@@ -7425,7 +7425,7 @@
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B288" t="s">
         <v>6</v>
@@ -7448,7 +7448,7 @@
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
-        <v>43937</v>
+        <v>43936</v>
       </c>
       <c r="B289" t="s">
         <v>7</v>
@@ -7467,6 +7467,190 @@
       </c>
       <c r="I289">
         <v>402</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B290" t="s">
+        <v>1</v>
+      </c>
+      <c r="C290">
+        <v>436</v>
+      </c>
+      <c r="D290">
+        <v>186</v>
+      </c>
+      <c r="E290">
+        <v>35</v>
+      </c>
+      <c r="G290">
+        <v>39</v>
+      </c>
+      <c r="I290">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B291" t="s">
+        <v>2</v>
+      </c>
+      <c r="C291">
+        <v>1110</v>
+      </c>
+      <c r="D291">
+        <v>466</v>
+      </c>
+      <c r="E291">
+        <v>73</v>
+      </c>
+      <c r="G291">
+        <v>71</v>
+      </c>
+      <c r="I291">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B292" t="s">
+        <v>3</v>
+      </c>
+      <c r="C292">
+        <v>1259</v>
+      </c>
+      <c r="D292">
+        <v>486</v>
+      </c>
+      <c r="E292">
+        <v>64</v>
+      </c>
+      <c r="G292">
+        <v>70</v>
+      </c>
+      <c r="I292">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B293" t="s">
+        <v>4</v>
+      </c>
+      <c r="C293">
+        <v>1956</v>
+      </c>
+      <c r="D293">
+        <v>1018</v>
+      </c>
+      <c r="E293">
+        <v>117</v>
+      </c>
+      <c r="G293">
+        <v>191</v>
+      </c>
+      <c r="I293">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B294" t="s">
+        <v>11</v>
+      </c>
+      <c r="C294">
+        <v>352</v>
+      </c>
+      <c r="D294">
+        <v>201</v>
+      </c>
+      <c r="E294">
+        <v>29</v>
+      </c>
+      <c r="G294">
+        <v>29</v>
+      </c>
+      <c r="I294">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B295" t="s">
+        <v>5</v>
+      </c>
+      <c r="C295">
+        <v>1233</v>
+      </c>
+      <c r="D295">
+        <v>612</v>
+      </c>
+      <c r="E295">
+        <v>62</v>
+      </c>
+      <c r="G295">
+        <v>129</v>
+      </c>
+      <c r="I295">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B296" t="s">
+        <v>6</v>
+      </c>
+      <c r="C296">
+        <v>2429</v>
+      </c>
+      <c r="D296">
+        <v>1317</v>
+      </c>
+      <c r="E296">
+        <v>157</v>
+      </c>
+      <c r="G296">
+        <v>214</v>
+      </c>
+      <c r="I296">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>43937</v>
+      </c>
+      <c r="B297" t="s">
+        <v>7</v>
+      </c>
+      <c r="C297">
+        <v>2278</v>
+      </c>
+      <c r="D297">
+        <v>1012</v>
+      </c>
+      <c r="E297">
+        <v>138</v>
+      </c>
+      <c r="G297">
+        <v>197</v>
+      </c>
+      <c r="I297">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -7495,43 +7679,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
       </c>
-      <c r="K1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7829,10 +8013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:F21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7846,19 +8030,19 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
@@ -7866,459 +8050,505 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43918</v>
+        <v>43916</v>
       </c>
       <c r="B2">
-        <v>20791</v>
+        <v>18592</v>
       </c>
       <c r="C2">
-        <v>4277</v>
+        <v>3793</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43919</v>
+        <v>43917</v>
       </c>
       <c r="B3">
-        <v>21235</v>
+        <v>20791</v>
       </c>
       <c r="C3">
-        <v>4682</v>
+        <v>4277</v>
       </c>
       <c r="D3">
         <f>B3-B2</f>
-        <v>444</v>
+        <v>2199</v>
       </c>
       <c r="E3">
         <f>C3-C2</f>
-        <v>405</v>
+        <v>484</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F6" si="0">E3/D3</f>
-        <v>0.91216216216216217</v>
+        <f t="shared" ref="F3" si="0">E3/D3</f>
+        <v>0.220100045475216</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43920</v>
+        <v>43918</v>
       </c>
       <c r="B4">
-        <v>23967</v>
+        <v>21235</v>
       </c>
       <c r="C4">
-        <v>5405</v>
+        <v>4682</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D6" si="1">B4-B3</f>
-        <v>2732</v>
+        <f>B4-B3</f>
+        <v>444</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E6" si="2">C4-C3</f>
-        <v>723</v>
+        <f>C4-C3</f>
+        <v>405</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>0.26464128843338214</v>
+        <f t="shared" ref="F4:F7" si="1">E4/D4</f>
+        <v>0.91216216216216217</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43921</v>
+        <v>43919</v>
       </c>
       <c r="B5">
-        <v>24850</v>
+        <v>23967</v>
       </c>
       <c r="C5">
-        <v>5818</v>
+        <v>5405</v>
       </c>
       <c r="D5">
+        <f t="shared" ref="D5:D7" si="2">B5-B4</f>
+        <v>2732</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E7" si="3">C5-C4</f>
+        <v>723</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="1"/>
-        <v>883</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="2"/>
-        <v>413</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>0.46772366930917325</v>
+        <v>0.26464128843338214</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43922</v>
+        <v>43920</v>
       </c>
       <c r="B6">
-        <v>26813</v>
+        <v>24850</v>
       </c>
       <c r="C6">
-        <v>6392</v>
+        <v>5818</v>
       </c>
       <c r="D6">
+        <f t="shared" si="2"/>
+        <v>883</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>413</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="1"/>
-        <v>1963</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>574</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0.29240957717778909</v>
+        <v>0.46772366930917325</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43923</v>
+        <v>43921</v>
       </c>
       <c r="B7">
-        <v>28863</v>
+        <v>26813</v>
       </c>
       <c r="C7">
-        <v>6972</v>
+        <v>6392</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7" si="3">B7-B6</f>
-        <v>2050</v>
+        <f t="shared" si="2"/>
+        <v>1963</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E7" si="4">C7-C6</f>
-        <v>580</v>
+        <f t="shared" si="3"/>
+        <v>574</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7" si="5">E7/D7</f>
-        <v>0.28292682926829266</v>
+        <f t="shared" si="1"/>
+        <v>0.29240957717778909</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43924</v>
+        <v>43922</v>
       </c>
       <c r="B8">
-        <v>30679</v>
+        <v>28863</v>
       </c>
       <c r="C8">
-        <v>7374</v>
+        <v>6972</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8" si="6">B8-B7</f>
-        <v>1816</v>
+        <f t="shared" ref="D8" si="4">B8-B7</f>
+        <v>2050</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8" si="7">C8-C7</f>
-        <v>402</v>
+        <f t="shared" ref="E8" si="5">C8-C7</f>
+        <v>580</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8" si="8">E8/D8</f>
-        <v>0.22136563876651982</v>
+        <f t="shared" ref="F8" si="6">E8/D8</f>
+        <v>0.28292682926829266</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43925</v>
+        <v>43923</v>
       </c>
       <c r="B9">
-        <v>32320</v>
+        <v>30679</v>
       </c>
       <c r="C9">
-        <v>7869</v>
+        <v>7374</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9" si="9">B9-B8</f>
-        <v>1641</v>
+        <f t="shared" ref="D9" si="7">B9-B8</f>
+        <v>1816</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9" si="10">C9-C8</f>
-        <v>495</v>
+        <f t="shared" ref="E9" si="8">C9-C8</f>
+        <v>402</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9" si="11">E9/D9</f>
-        <v>0.3016453382084095</v>
+        <f t="shared" ref="F9" si="9">E9/D9</f>
+        <v>0.22136563876651982</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43926</v>
+        <v>43924</v>
       </c>
       <c r="B10">
-        <v>34096</v>
+        <v>32320</v>
       </c>
       <c r="C10">
-        <v>8301</v>
+        <v>7869</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10" si="12">B10-B9</f>
-        <v>1776</v>
+        <f t="shared" ref="D10" si="10">B10-B9</f>
+        <v>1641</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10" si="13">C10-C9</f>
-        <v>432</v>
+        <f t="shared" ref="E10" si="11">C10-C9</f>
+        <v>495</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10" si="14">E10/D10</f>
-        <v>0.24324324324324326</v>
+        <f t="shared" ref="F10" si="12">E10/D10</f>
+        <v>0.3016453382084095</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43927</v>
+        <v>43925</v>
       </c>
       <c r="B11">
-        <v>34592</v>
+        <v>34096</v>
       </c>
       <c r="C11">
-        <v>8581</v>
+        <v>8301</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11" si="15">B11-B10</f>
-        <v>496</v>
+        <f t="shared" ref="D11" si="13">B11-B10</f>
+        <v>1776</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11" si="16">C11-C10</f>
-        <v>280</v>
+        <f t="shared" ref="E11" si="14">C11-C10</f>
+        <v>432</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11" si="17">E11/D11</f>
-        <v>0.56451612903225812</v>
+        <f t="shared" ref="F11" si="15">E11/D11</f>
+        <v>0.24324324324324326</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43928</v>
+        <v>43926</v>
       </c>
       <c r="B12">
-        <v>35182</v>
+        <v>34592</v>
       </c>
       <c r="C12">
-        <v>8767</v>
+        <v>8581</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12" si="18">B12-B11</f>
-        <v>590</v>
+        <f t="shared" ref="D12" si="16">B12-B11</f>
+        <v>496</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12" si="19">C12-C11</f>
-        <v>186</v>
+        <f t="shared" ref="E12" si="17">C12-C11</f>
+        <v>280</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12" si="20">E12/D12</f>
-        <v>0.31525423728813562</v>
-      </c>
-      <c r="G12" t="s">
-        <v>94</v>
+        <f t="shared" ref="F12" si="18">E12/D12</f>
+        <v>0.56451612903225812</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43929</v>
+        <v>43927</v>
       </c>
       <c r="B13">
-        <v>36635</v>
+        <v>35182</v>
       </c>
       <c r="C13">
-        <v>8997</v>
+        <v>8767</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13" si="21">B13-B12</f>
-        <v>1453</v>
+        <f t="shared" ref="D13" si="19">B13-B12</f>
+        <v>590</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13" si="22">C13-C12</f>
-        <v>230</v>
+        <f t="shared" ref="E13" si="20">C13-C12</f>
+        <v>186</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13" si="23">E13/D13</f>
-        <v>0.15829318651066759</v>
+        <f t="shared" ref="F13" si="21">E13/D13</f>
+        <v>0.31525423728813562</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>43930</v>
+        <v>43928</v>
       </c>
       <c r="B14">
-        <v>38223</v>
+        <v>36635</v>
       </c>
       <c r="C14">
-        <v>9261</v>
+        <v>8997</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14" si="24">B14-B13</f>
-        <v>1588</v>
+        <f t="shared" ref="D14" si="22">B14-B13</f>
+        <v>1453</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14" si="25">C14-C13</f>
-        <v>264</v>
+        <f t="shared" ref="E14" si="23">C14-C13</f>
+        <v>230</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14" si="26">E14/D14</f>
-        <v>0.16624685138539042</v>
+        <f t="shared" ref="F14" si="24">E14/D14</f>
+        <v>0.15829318651066759</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>43931</v>
+        <v>43929</v>
       </c>
       <c r="B15">
-        <v>39820</v>
+        <v>38223</v>
       </c>
       <c r="C15">
-        <v>9510</v>
+        <v>9261</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:D16" si="27">B15-B14</f>
-        <v>1597</v>
+        <f t="shared" ref="D15" si="25">B15-B14</f>
+        <v>1588</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E16" si="28">C15-C14</f>
-        <v>249</v>
+        <f t="shared" ref="E15" si="26">C15-C14</f>
+        <v>264</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F16" si="29">E15/D15</f>
-        <v>0.15591734502191609</v>
+        <f t="shared" ref="F15" si="27">E15/D15</f>
+        <v>0.16624685138539042</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>43932</v>
+        <v>43930</v>
       </c>
       <c r="B16">
-        <v>40628</v>
+        <v>39820</v>
       </c>
       <c r="C16">
-        <v>9712</v>
+        <v>9510</v>
       </c>
       <c r="D16">
-        <f t="shared" si="27"/>
-        <v>808</v>
+        <f t="shared" ref="D16:D17" si="28">B16-B15</f>
+        <v>1597</v>
       </c>
       <c r="E16">
-        <f t="shared" si="28"/>
-        <v>202</v>
+        <f t="shared" ref="E16:E17" si="29">C16-C15</f>
+        <v>249</v>
       </c>
       <c r="F16">
-        <f t="shared" si="29"/>
-        <v>0.25</v>
+        <f t="shared" ref="F16:F17" si="30">E16/D16</f>
+        <v>0.15591734502191609</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>43933</v>
+        <v>43931</v>
       </c>
       <c r="B17">
-        <v>41227</v>
+        <v>40628</v>
       </c>
       <c r="C17">
-        <v>10006</v>
+        <v>9712</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17" si="30">B17-B16</f>
-        <v>599</v>
+        <f t="shared" si="28"/>
+        <v>808</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17" si="31">C17-C16</f>
-        <v>294</v>
+        <f t="shared" si="29"/>
+        <v>202</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17" si="32">E17/D17</f>
-        <v>0.49081803005008345</v>
+        <f t="shared" si="30"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>43934</v>
+        <v>43932</v>
       </c>
       <c r="B18">
-        <v>41749</v>
+        <v>41227</v>
       </c>
       <c r="C18">
-        <v>10187</v>
+        <v>10006</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18" si="33">B18-B17</f>
-        <v>522</v>
+        <f t="shared" ref="D18" si="31">B18-B17</f>
+        <v>599</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18" si="34">C18-C17</f>
-        <v>181</v>
+        <f t="shared" ref="E18" si="32">C18-C17</f>
+        <v>294</v>
       </c>
       <c r="F18">
-        <f t="shared" ref="F18" si="35">E18/D18</f>
-        <v>0.34674329501915707</v>
+        <f t="shared" ref="F18" si="33">E18/D18</f>
+        <v>0.49081803005008345</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>43935</v>
+        <v>43933</v>
       </c>
       <c r="B19">
-        <v>42363</v>
+        <v>41749</v>
       </c>
       <c r="C19">
-        <v>10306</v>
+        <v>10187</v>
       </c>
       <c r="D19">
-        <f t="shared" ref="D19" si="36">B19-B18</f>
-        <v>614</v>
+        <f t="shared" ref="D19" si="34">B19-B18</f>
+        <v>522</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="E19" si="37">C19-C18</f>
-        <v>119</v>
+        <f t="shared" ref="E19" si="35">C19-C18</f>
+        <v>181</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19" si="38">E19/D19</f>
-        <v>0.19381107491856678</v>
-      </c>
-      <c r="G19" t="s">
-        <v>95</v>
+        <f t="shared" ref="F19" si="36">E19/D19</f>
+        <v>0.34674329501915707</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>43936</v>
+        <v>43934</v>
       </c>
       <c r="B20">
-        <v>43625</v>
+        <v>42363</v>
       </c>
       <c r="C20">
-        <v>10595</v>
+        <v>10306</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20" si="39">B20-B19</f>
-        <v>1262</v>
+        <f t="shared" ref="D20" si="37">B20-B19</f>
+        <v>614</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20" si="40">C20-C19</f>
-        <v>289</v>
+        <f t="shared" ref="E20" si="38">C20-C19</f>
+        <v>119</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20" si="41">E20/D20</f>
-        <v>0.22900158478605387</v>
+        <f t="shared" ref="F20" si="39">E20/D20</f>
+        <v>0.19381107491856678</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
+        <v>43935</v>
+      </c>
+      <c r="B21">
+        <v>43625</v>
+      </c>
+      <c r="C21">
+        <v>10595</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21" si="40">B21-B20</f>
+        <v>1262</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21" si="41">C21-C20</f>
+        <v>289</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21" si="42">E21/D21</f>
+        <v>0.22900158478605387</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43936</v>
+      </c>
+      <c r="B22">
+        <v>44598</v>
+      </c>
+      <c r="C22">
+        <v>10807</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22" si="43">B22-B21</f>
+        <v>973</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22" si="44">C22-C21</f>
+        <v>212</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22" si="45">E22/D22</f>
+        <v>0.21788283658787255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>43937</v>
       </c>
-      <c r="B21">
-        <v>44598</v>
-      </c>
-      <c r="C21">
-        <v>10807</v>
-      </c>
-      <c r="D21">
-        <f t="shared" ref="D21" si="42">B21-B20</f>
-        <v>973</v>
-      </c>
-      <c r="E21">
-        <f t="shared" ref="E21" si="43">C21-C20</f>
-        <v>212</v>
-      </c>
-      <c r="F21">
-        <f t="shared" ref="F21" si="44">E21/D21</f>
-        <v>0.21788283658787255</v>
+      <c r="B23">
+        <v>45675</v>
+      </c>
+      <c r="C23">
+        <v>11053</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23" si="46">B23-B22</f>
+        <v>1077</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23" si="47">C23-C22</f>
+        <v>246</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23" si="48">E23/D23</f>
+        <v>0.22841225626740946</v>
       </c>
     </row>
   </sheetData>
@@ -8345,15 +8575,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>157</v>
@@ -8361,7 +8591,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>101</v>
@@ -8369,7 +8599,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5">
         <v>67</v>
@@ -8377,7 +8607,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>174</v>
@@ -8385,7 +8615,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>118</v>
@@ -8393,7 +8623,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>46</v>
@@ -8401,7 +8631,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>109</v>
@@ -8409,7 +8639,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>93</v>
@@ -8417,7 +8647,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>67</v>
@@ -8425,7 +8655,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>73</v>
@@ -8433,7 +8663,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>358</v>
@@ -8441,7 +8671,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>295</v>
@@ -8449,7 +8679,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>311</v>
@@ -8457,7 +8687,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>150</v>
@@ -8465,7 +8695,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>364</v>
@@ -8473,7 +8703,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>70</v>
@@ -8481,7 +8711,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>458</v>
@@ -8489,7 +8719,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>366</v>
@@ -8497,7 +8727,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>626</v>
@@ -8505,7 +8735,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>40</v>
@@ -8513,7 +8743,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>145</v>
@@ -8521,7 +8751,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>425</v>
@@ -8529,7 +8759,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>129</v>
@@ -8537,7 +8767,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <v>294</v>
@@ -8545,7 +8775,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26">
         <v>79</v>
@@ -8553,7 +8783,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>209</v>
@@ -8561,7 +8791,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28">
         <v>1106</v>
@@ -8569,7 +8799,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>666</v>
@@ -8577,7 +8807,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30">
         <v>153</v>
@@ -8585,7 +8815,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31">
         <v>828</v>
@@ -8593,7 +8823,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32">
         <v>127</v>
@@ -8601,7 +8831,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33">
         <v>115</v>
@@ -8609,7 +8839,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34">
         <v>150</v>
@@ -8617,7 +8847,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" s="5">
         <v>112</v>
@@ -8646,25 +8876,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
-        <v>63</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
         <v>92</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -8672,7 +8902,7 @@
         <v>3004</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -8712,7 +8942,7 @@
         <v>3012</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -8732,7 +8962,7 @@
         <v>3013</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -8752,7 +8982,7 @@
         <v>3003</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -8772,7 +9002,7 @@
         <v>3022</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -8812,7 +9042,7 @@
         <v>3049</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -8832,7 +9062,7 @@
         <v>3043</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -8852,7 +9082,7 @@
         <v>3026</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -8892,7 +9122,7 @@
         <v>3029</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8912,7 +9142,7 @@
         <v>3023</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -8932,7 +9162,7 @@
         <v>3048</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -8952,7 +9182,7 @@
         <v>3030</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -8992,7 +9222,7 @@
         <v>3045</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -9012,7 +9242,7 @@
         <v>3034</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -9032,7 +9262,7 @@
         <v>3001</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -9052,7 +9282,7 @@
         <v>3032</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -9072,7 +9302,7 @@
         <v>3011</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -9092,7 +9322,7 @@
         <v>3033</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -9132,7 +9362,7 @@
         <v>3056</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -9152,7 +9382,7 @@
         <v>3050</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -9172,7 +9402,7 @@
         <v>3052</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -9212,7 +9442,7 @@
         <v>3047</v>
       </c>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -9232,7 +9462,7 @@
         <v>3051</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -9252,7 +9482,7 @@
         <v>3002</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -9272,7 +9502,7 @@
         <v>3062</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -9292,7 +9522,7 @@
         <v>3009</v>
       </c>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -9312,7 +9542,7 @@
         <v>3021</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -9345,7 +9575,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -9370,43 +9600,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
       </c>
-      <c r="K1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -9719,43 +9949,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
       </c>
-      <c r="K1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -10068,43 +10298,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
       </c>
-      <c r="K1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -10417,43 +10647,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
         <v>96</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>97</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>100</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
       </c>
-      <c r="K1" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>